<commit_message>
update history home and hd again
</commit_message>
<xml_diff>
--- a/Git_History_Between_Home_HD.xlsx
+++ b/Git_History_Between_Home_HD.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Merge message need to edit , save and close before pull operation started</t>
   </si>
@@ -34,6 +34,15 @@
   </si>
   <si>
     <t>commit the change for hdfile1.txt</t>
+  </si>
+  <si>
+    <t>general commit without enter 'message' - you got prompted by message which I entered " go ahead"</t>
+  </si>
+  <si>
+    <t>after save and close the file, commit is done</t>
+  </si>
+  <si>
+    <t>go ahead</t>
   </si>
 </sst>
 </file>
@@ -397,6 +406,154 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>347</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>579011</xdr:colOff>
+      <xdr:row>391</xdr:row>
+      <xdr:rowOff>182723</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="640080" y="63459360"/>
+          <a:ext cx="5699651" cy="8229443"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>544830</xdr:colOff>
+      <xdr:row>371</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>375</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rounded Rectangle 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="544830" y="67974210"/>
+          <a:ext cx="3950970" cy="605790"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-AU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>370</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>373</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="502920" y="67760850"/>
+          <a:ext cx="1668780" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -690,10 +847,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:C295"/>
+  <dimension ref="A2:C370"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
-      <selection activeCell="B296" sqref="B296"/>
+    <sheetView tabSelected="1" topLeftCell="A367" workbookViewId="0">
+      <selection activeCell="M374" sqref="M374"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -728,6 +885,21 @@
         <v>5</v>
       </c>
     </row>
+    <row r="345" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B345" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="346" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B346" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A370" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>